<commit_message>
Added level data converter and two levels to test it
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0BDC62C-C7F0-43A4-B8A9-7E3CD62E61E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E951E37-AFF1-43E0-A1DC-E14085F0F001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad6" sheetId="6" r:id="rId1"/>
-    <sheet name="01" sheetId="1" r:id="rId2"/>
-    <sheet name="02" sheetId="2" r:id="rId3"/>
-    <sheet name="03" sheetId="3" r:id="rId4"/>
+    <sheet name="base" sheetId="3" r:id="rId1"/>
+    <sheet name="info" sheetId="6" r:id="rId2"/>
+    <sheet name="01" sheetId="1" r:id="rId3"/>
+    <sheet name="02" sheetId="2" r:id="rId4"/>
     <sheet name="04" sheetId="4" r:id="rId5"/>
     <sheet name="05" sheetId="5" r:id="rId6"/>
   </sheets>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="22">
   <si>
     <t>D</t>
   </si>
@@ -74,6 +74,39 @@
   </si>
   <si>
     <t>Totaal</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>clr</t>
+  </si>
+  <si>
+    <t>r/c</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
@@ -786,7 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -861,9 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -918,7 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1047,7 +1077,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1104,14 +1134,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1425,28 +1456,281 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95440412-A2B7-43E5-A6C1-1A36CF91A08F}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="27"/>
+    <col min="2" max="15" width="3.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="28">
+        <v>0</v>
+      </c>
+      <c r="C1" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1" s="28">
+        <v>2</v>
+      </c>
+      <c r="E1" s="28">
+        <v>3</v>
+      </c>
+      <c r="F1" s="28">
+        <v>4</v>
+      </c>
+      <c r="G1" s="28">
+        <v>5</v>
+      </c>
+      <c r="H1" s="28">
+        <v>6</v>
+      </c>
+      <c r="I1" s="28">
+        <v>7</v>
+      </c>
+      <c r="J1" s="28">
+        <v>8</v>
+      </c>
+      <c r="K1" s="28">
+        <v>9</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1B7977-7B33-4887-94B8-2677514B6F62}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="111" t="s">
+      <c r="D1" s="112" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="112"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="113"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1454,33 +1738,32 @@
         <f>'01'!Q2</f>
         <v>27</v>
       </c>
-      <c r="D2" s="113">
+      <c r="D2" s="110">
         <f>SUM(B:B)</f>
-        <v>315</v>
-      </c>
-      <c r="E2" s="114" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" s="111" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <f>'02'!Q2</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <f>'03'!Q2</f>
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1488,8 +1771,14 @@
         <f>'04'!Q2</f>
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="114" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1497,53 +1786,77 @@
         <f>'05'!Q2</f>
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="114" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="114" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="114" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="114" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1607,18 +1920,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BB428C-4651-4B9F-9821-E588F1484CFA}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14:P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="27"/>
     <col min="2" max="15" width="3.5546875" customWidth="1"/>
+    <col min="16" max="16" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1701,10 +2015,10 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1723,16 +2037,16 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -1749,16 +2063,16 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="20" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J5" s="26" t="s">
         <v>2</v>
@@ -1850,22 +2164,22 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -1882,16 +2196,16 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -1910,10 +2224,10 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1941,23 +2255,356 @@
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
     </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="P14" t="str">
+        <f>CONCATENATE(".db #$", C14, B14, ", #%", IF(E14="R", "0", "1"),  DEC2BIN(D14-1,2), VLOOKUP(F14, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G14,3))</f>
+        <v>.db #$61, #%00100001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="P15" t="str">
+        <f>CONCATENATE(".db #$", C15, B15, ", #%", IF(E15="R", "0", "1"),  DEC2BIN(D15-1,2), VLOOKUP(F15, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G15,3))</f>
+        <v>.db #$52, #%01100001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="P16" t="str">
+        <f>CONCATENATE(".db #$", C16, B16, ", #%", IF(E16="R", "0", "1"),  DEC2BIN(D16-1,2), VLOOKUP(F16, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G16,3))</f>
+        <v>.db #$43, #%01100010</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="P17" t="str">
+        <f>CONCATENATE(".db #$", C17, B17, ", #%", IF(E17="R", "0", "1"),  DEC2BIN(D17-1,2), VLOOKUP(F17, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G17,3))</f>
+        <v>.db #$83, #%00000010</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="P18" t="str">
+        <f>CONCATENATE(".db #$", C18, B18, ", #%", IF(E18="R", "0", "1"),  DEC2BIN(D18-1,2), VLOOKUP(F18, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G18,3))</f>
+        <v>.db #$93, #%00010010</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="str">
+        <f>CONCATENATE(".db #$", C19, B19, ", #%", IF(E19="R", "0", "1"),  DEC2BIN(D19-1,2), VLOOKUP(F19, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G19,3))</f>
+        <v>.db #$34, #%01111000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="str">
+        <f>CONCATENATE(".db #$", C20, B20, ", #%", IF(E20="R", "0", "1"),  DEC2BIN(D20-1,2), VLOOKUP(F20, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G20,3))</f>
+        <v>.db #$74, #%01111000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="str">
+        <f>CONCATENATE(".db #$", C21, B21, ", #%", IF(E21="R", "0", "1"),  DEC2BIN(D21-1,2), VLOOKUP(F21, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G21,3))</f>
+        <v>.db #$35, #%01111000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="P22" t="str">
+        <f>CONCATENATE(".db #$", C22, B22, ", #%", IF(E22="R", "0", "1"),  DEC2BIN(D22-1,2), VLOOKUP(F22, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G22,3))</f>
+        <v>.db #$75, #%01111000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="P23" t="str">
+        <f>CONCATENATE(".db #$", C23, B23, ", #%", IF(E23="R", "0", "1"),  DEC2BIN(D23-1,2), VLOOKUP(F23, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G23,3))</f>
+        <v>.db #$46, #%01100010</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="P24" t="str">
+        <f>CONCATENATE(".db #$", C24, B24, ", #%", IF(E24="R", "0", "1"),  DEC2BIN(D24-1,2), VLOOKUP(F24, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G24,3))</f>
+        <v>.db #$86, #%00100010</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="P25" t="str">
+        <f>CONCATENATE(".db #$", C25, B25, ", #%", IF(E25="R", "0", "1"),  DEC2BIN(D25-1,2), VLOOKUP(F25, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G25,3))</f>
+        <v>.db #$57, #%01100001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="P26" t="str">
+        <f>CONCATENATE(".db #$", C26, B26, ", #%", IF(E26="R", "0", "1"),  DEC2BIN(D26-1,2), VLOOKUP(F26, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G26,3))</f>
+        <v>.db #$68, #%00100001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8571E8-FA34-41DE-BC66-C61EF0B5623D}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14:P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="27"/>
     <col min="2" max="15" width="3.5546875" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2020,12 +2667,12 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="47" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="3"/>
       <c r="Q2">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R2" t="s">
         <v>7</v>
@@ -2036,40 +2683,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="35" t="s">
+      <c r="C3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="34" t="s">
         <v>4</v>
       </c>
       <c r="O3" s="6"/>
@@ -2079,40 +2726,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" s="38" t="s">
+      <c r="C4" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="37" t="s">
         <v>6</v>
       </c>
       <c r="O4" s="6"/>
@@ -2122,18 +2769,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="39" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="38" t="s">
         <v>5</v>
       </c>
       <c r="O5" s="6"/>
@@ -2146,37 +2793,37 @@
       <c r="C6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="42" t="s">
+      <c r="D6" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="41" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="6"/>
@@ -2186,40 +2833,40 @@
         <v>5</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="38" t="s">
+      <c r="C7" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="O7" s="6"/>
@@ -2229,17 +2876,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="6"/>
     </row>
@@ -2248,7 +2895,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="10" t="s">
@@ -2291,40 +2938,40 @@
         <v>8</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" s="47" t="s">
+      <c r="C10" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="46" t="s">
         <v>6</v>
       </c>
       <c r="O10" s="6"/>
@@ -2348,264 +2995,649 @@
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95440412-A2B7-43E5-A6C1-1A36CF91A08F}">
-  <dimension ref="A1:R11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="27"/>
-    <col min="2" max="15" width="3.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="28">
-        <v>0</v>
-      </c>
-      <c r="C1" s="28">
-        <v>1</v>
-      </c>
-      <c r="D1" s="28">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="P14" t="str">
+        <f>CONCATENATE(".db #$", C14, B14, ", #%", IF(E14="R", "0", "1"),  DEC2BIN(D14-1,2), VLOOKUP(F14, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G14,3))</f>
+        <v>.db #$C0, #%00001001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15">
         <v>2</v>
       </c>
-      <c r="E1" s="28">
+      <c r="P15" t="str">
+        <f>CONCATENATE(".db #$", C15, B15, ", #%", IF(E15="R", "0", "1"),  DEC2BIN(D15-1,2), VLOOKUP(F15, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G15,3))</f>
+        <v>.db #$11, #%00010010</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="P16" t="str">
+        <f>CONCATENATE(".db #$", C16, B16, ", #%", IF(E16="R", "0", "1"),  DEC2BIN(D16-1,2), VLOOKUP(F16, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G16,3))</f>
+        <v>.db #$21, #%01100001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="P17" t="str">
+        <f>CONCATENATE(".db #$", C17, B17, ", #%", IF(E17="R", "0", "1"),  DEC2BIN(D17-1,2), VLOOKUP(F17, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G17,3))</f>
+        <v>.db #$61, #%01100001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28">
-        <v>4</v>
-      </c>
-      <c r="G1" s="28">
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="P18" t="str">
+        <f>CONCATENATE(".db #$", C18, B18, ", #%", IF(E18="R", "0", "1"),  DEC2BIN(D18-1,2), VLOOKUP(F18, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G18,3))</f>
+        <v>.db #$A1, #%01000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="P19" t="str">
+        <f>CONCATENATE(".db #$", C19, B19, ", #%", IF(E19="R", "0", "1"),  DEC2BIN(D19-1,2), VLOOKUP(F19, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G19,3))</f>
+        <v>.db #$12, #%01100111</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
         <v>5</v>
       </c>
-      <c r="H1" s="28">
-        <v>6</v>
-      </c>
-      <c r="I1" s="28">
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20">
         <v>7</v>
       </c>
-      <c r="J1" s="28">
+      <c r="P20" t="str">
+        <f>CONCATENATE(".db #$", C20, B20, ", #%", IF(E20="R", "0", "1"),  DEC2BIN(D20-1,2), VLOOKUP(F20, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G20,3))</f>
+        <v>.db #$52, #%01100111</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="P21" t="str">
+        <f>CONCATENATE(".db #$", C21, B21, ", #%", IF(E21="R", "0", "1"),  DEC2BIN(D21-1,2), VLOOKUP(F21, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G21,3))</f>
+        <v>.db #$92, #%01100111</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="P22" t="str">
+        <f>CONCATENATE(".db #$", C22, B22, ", #%", IF(E22="R", "0", "1"),  DEC2BIN(D22-1,2), VLOOKUP(F22, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G22,3))</f>
+        <v>.db #$C3, #%00001010</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="P23" t="str">
+        <f>CONCATENATE(".db #$", C23, B23, ", #%", IF(E23="R", "0", "1"),  DEC2BIN(D23-1,2), VLOOKUP(F23, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G23,3))</f>
+        <v>.db #$14, #%00010011</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="P24" t="str">
+        <f>CONCATENATE(".db #$", C24, B24, ", #%", IF(E24="R", "0", "1"),  DEC2BIN(D24-1,2), VLOOKUP(F24, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G24,3))</f>
+        <v>.db #$24, #%01100010</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="P25" t="str">
+        <f>CONCATENATE(".db #$", C25, B25, ", #%", IF(E25="R", "0", "1"),  DEC2BIN(D25-1,2), VLOOKUP(F25, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G25,3))</f>
+        <v>.db #$64, #%01100010</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="P26" t="str">
+        <f>CONCATENATE(".db #$", C26, B26, ", #%", IF(E26="R", "0", "1"),  DEC2BIN(D26-1,2), VLOOKUP(F26, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G26,3))</f>
+        <v>.db #$A4, #%01000010</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>7</v>
+      </c>
+      <c r="P27" t="str">
+        <f>CONCATENATE(".db #$", C27, B27, ", #%", IF(E27="R", "0", "1"),  DEC2BIN(D27-1,2), VLOOKUP(F27, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G27,3))</f>
+        <v>.db #$15, #%01100111</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>7</v>
+      </c>
+      <c r="P28" t="str">
+        <f>CONCATENATE(".db #$", C28, B28, ", #%", IF(E28="R", "0", "1"),  DEC2BIN(D28-1,2), VLOOKUP(F28, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G28,3))</f>
+        <v>.db #$55, #%01100111</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="P29" t="str">
+        <f>CONCATENATE(".db #$", C29, B29, ", #%", IF(E29="R", "0", "1"),  DEC2BIN(D29-1,2), VLOOKUP(F29, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G29,3))</f>
+        <v>.db #$95, #%01100111</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="P30" t="str">
+        <f>CONCATENATE(".db #$", C30, B30, ", #%", IF(E30="R", "0", "1"),  DEC2BIN(D30-1,2), VLOOKUP(F30, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G30,3))</f>
+        <v>.db #$17, #%00010001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="P31" t="str">
+        <f>CONCATENATE(".db #$", C31, B31, ", #%", IF(E31="R", "0", "1"),  DEC2BIN(D31-1,2), VLOOKUP(F31, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G31,3))</f>
+        <v>.db #$27, #%01100011</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="P32" t="str">
+        <f>CONCATENATE(".db #$", C32, B32, ", #%", IF(E32="R", "0", "1"),  DEC2BIN(D32-1,2), VLOOKUP(F32, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G32,3))</f>
+        <v>.db #$67, #%01100011</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="P33" t="str">
+        <f>CONCATENATE(".db #$", C33, B33, ", #%", IF(E33="R", "0", "1"),  DEC2BIN(D33-1,2), VLOOKUP(F33, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G33,3))</f>
+        <v>.db #$A7, #%01000011</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B34">
         <v>8</v>
       </c>
-      <c r="K1" s="28">
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="P34" t="str">
+        <f>CONCATENATE(".db #$", C34, B34, ", #%", IF(E34="R", "0", "1"),  DEC2BIN(D34-1,2), VLOOKUP(F34, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G34,3))</f>
+        <v>.db #$38, #%01111000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
         <v>9</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="D35">
         <v>3</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="P35" t="str">
+        <f>CONCATENATE(".db #$", C35, B35, ", #%", IF(E35="R", "0", "1"),  DEC2BIN(D35-1,2), VLOOKUP(F35, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G35,3))</f>
+        <v>.db #$98, #%01011000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
         <v>2</v>
       </c>
-      <c r="N1" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3"/>
-      <c r="Q2">
-        <v>55</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="6"/>
-    </row>
-    <row r="4" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
+      <c r="P36" t="str">
+        <f>CONCATENATE(".db #$", C36, B36, ", #%", IF(E36="R", "0", "1"),  DEC2BIN(D36-1,2), VLOOKUP(F36, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G36,3))</f>
+        <v>.db #$18, #%00100111</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
+      <c r="P37" t="str">
+        <f>CONCATENATE(".db #$", C37, B37, ", #%", IF(E37="R", "0", "1"),  DEC2BIN(D37-1,2), VLOOKUP(F37, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G37,3))</f>
+        <v>.db #$48, #%00100111</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B38">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="1:18" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="29">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9"/>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>7</v>
+      </c>
+      <c r="P38" t="str">
+        <f>CONCATENATE(".db #$", C38, B38, ", #%", IF(E38="R", "0", "1"),  DEC2BIN(D38-1,2), VLOOKUP(F38, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G38,3))</f>
+        <v>.db #$78, #%00100111</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="P39" t="str">
+        <f>CONCATENATE(".db #$", C39, B39, ", #%", IF(E39="R", "0", "1"),  DEC2BIN(D39-1,2), VLOOKUP(F39, info!$H$5:$I$9, 2, FALSE), DEC2BIN(G39,3))</f>
+        <v>.db #$C8, #%00000111</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2674,20 +3706,20 @@
       <c r="A2" s="29">
         <v>0</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="72"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="Q2">
         <v>119</v>
       </c>
@@ -2699,172 +3731,172 @@
       <c r="A3" s="29">
         <v>1</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
       <c r="J3" s="26"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="62"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="61"/>
       <c r="N3" s="16"/>
-      <c r="O3" s="74"/>
+      <c r="O3" s="73"/>
     </row>
     <row r="4" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>2</v>
       </c>
-      <c r="B4" s="75"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="76"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="75"/>
     </row>
     <row r="5" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>3</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="48"/>
       <c r="N5" s="26"/>
-      <c r="O5" s="77"/>
+      <c r="O5" s="76"/>
     </row>
     <row r="6" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>4</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="17"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="54"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="53"/>
       <c r="J6" s="17"/>
       <c r="K6" s="25"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="78"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="77"/>
     </row>
     <row r="7" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>5</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="62"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="20"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="59"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="58"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="78"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="77"/>
     </row>
     <row r="8" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>6</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="55"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="54"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="52"/>
       <c r="H8" s="26"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="56"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="55"/>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="18"/>
-      <c r="O8" s="80"/>
+      <c r="O8" s="79"/>
     </row>
     <row r="9" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>7</v>
       </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="58"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="57"/>
       <c r="N9" s="26"/>
-      <c r="O9" s="82"/>
+      <c r="O9" s="81"/>
     </row>
     <row r="10" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>8</v>
       </c>
-      <c r="B10" s="83"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="52"/>
       <c r="I10" s="20"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="84"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="83"/>
     </row>
     <row r="11" spans="1:18" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>9</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="91"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="85"/>
+      <c r="O11" s="90"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2937,24 +3969,24 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="104" t="s">
+      <c r="I2" s="103" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="107" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="108" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="109" t="s">
+      <c r="M2" s="106" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="107" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="108" t="s">
         <v>4</v>
       </c>
       <c r="Q2">
@@ -2969,25 +4001,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="93" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" s="74" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="92" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="73" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2996,29 +4028,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="94" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="93" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" s="110" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="109" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3026,44 +4058,44 @@
       <c r="A5" s="29">
         <v>3</v>
       </c>
-      <c r="B5" s="97" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="105" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="106" t="s">
+      <c r="B5" s="96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="104" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="105" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3072,17 +4104,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="6"/>
     </row>
@@ -3090,10 +4122,10 @@
       <c r="A7" s="29">
         <v>5</v>
       </c>
-      <c r="B7" s="98" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="30"/>
+      <c r="B7" s="97" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="26" t="s">
         <v>4</v>
       </c>
@@ -3103,7 +4135,7 @@
       <c r="F7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="16" t="s">
         <v>4</v>
       </c>
@@ -3113,7 +4145,7 @@
       <c r="J7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="30"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="20" t="s">
         <v>4</v>
       </c>
@@ -3129,30 +4161,30 @@
       <c r="A8" s="29">
         <v>6</v>
       </c>
-      <c r="B8" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="30"/>
+      <c r="B8" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="30"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="30"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5"/>
       <c r="N8" s="26" t="s">
         <v>4</v>
       </c>
@@ -3162,37 +4194,37 @@
       <c r="A9" s="29">
         <v>7</v>
       </c>
-      <c r="B9" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="30"/>
+      <c r="B9" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="16" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="53" t="s">
+      <c r="F9" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="52" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="95" t="s">
-        <v>4</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="63" t="s">
+      <c r="J9" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="62" t="s">
         <v>4</v>
       </c>
       <c r="O9" s="6"/>
@@ -3201,29 +4233,29 @@
       <c r="A10" s="29">
         <v>8</v>
       </c>
-      <c r="B10" s="81" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="30"/>
-      <c r="J10" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="95" t="s">
-        <v>4</v>
-      </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="53" t="s">
+      <c r="B10" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="52" t="s">
         <v>4</v>
       </c>
       <c r="O10" s="6"/>
@@ -3232,33 +4264,33 @@
       <c r="A11" s="29">
         <v>9</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="98" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="87" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="100" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="88" t="s">
+      <c r="H11" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="99" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="87" t="s">
         <v>4</v>
       </c>
       <c r="K11" s="8"/>
-      <c r="L11" s="101" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" s="102" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="103" t="s">
+      <c r="L11" s="100" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="102" t="s">
         <v>4</v>
       </c>
       <c r="O11" s="9"/>

</xml_diff>

<commit_message>
Fixed level 7 colors
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736B76B2-AC8B-458A-B0E2-55E393042DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB2C7B5-51A8-48A4-8950-7C24D0BCE732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -2590,9 +2590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA34367-0DD3-496D-9AFB-6A1C26D7B547}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="13" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P14" sqref="P14:P46"/>
+      <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20237,9 +20237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E74543B-0EF5-4872-B40B-688829014A48}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P45" sqref="P14:P45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20666,11 +20666,11 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P15" t="str">
         <f>CONCATENATE(".db #$", C15, B15, ", #%", IF(E15="R", "0", "1"),  DEC2BIN(D15-1,2), VLOOKUP(F15, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G15, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$01, #%11111100</v>
+        <v>.db #$01, #%11111010</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -20690,11 +20690,11 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P16" t="str">
         <f>CONCATENATE(".db #$", C16, B16, ", #%", IF(E16="R", "0", "1"),  DEC2BIN(D16-1,2), VLOOKUP(F16, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G16, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$12, #%10111100</v>
+        <v>.db #$12, #%10111010</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
@@ -20714,11 +20714,11 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P17" t="str">
         <f>CONCATENATE(".db #$", C17, B17, ", #%", IF(E17="R", "0", "1"),  DEC2BIN(D17-1,2), VLOOKUP(F17, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G17, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$23, #%11011100</v>
+        <v>.db #$23, #%11011010</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
@@ -20738,11 +20738,11 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P18" t="str">
         <f>CONCATENATE(".db #$", C18, B18, ", #%", IF(E18="R", "0", "1"),  DEC2BIN(D18-1,2), VLOOKUP(F18, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G18, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$34, #%11111100</v>
+        <v>.db #$34, #%11111010</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
@@ -20762,11 +20762,11 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P19" t="str">
         <f>CONCATENATE(".db #$", C19, B19, ", #%", IF(E19="R", "0", "1"),  DEC2BIN(D19-1,2), VLOOKUP(F19, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G19, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$05, #%11011100</v>
+        <v>.db #$05, #%11011010</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
@@ -20786,11 +20786,11 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P20" t="str">
         <f>CONCATENATE(".db #$", C20, B20, ", #%", IF(E20="R", "0", "1"),  DEC2BIN(D20-1,2), VLOOKUP(F20, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G20, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$15, #%11111100</v>
+        <v>.db #$15, #%11111010</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
@@ -20810,11 +20810,11 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P21" t="str">
         <f>CONCATENATE(".db #$", C21, B21, ", #%", IF(E21="R", "0", "1"),  DEC2BIN(D21-1,2), VLOOKUP(F21, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G21, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$45, #%10111100</v>
+        <v>.db #$45, #%10111010</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
@@ -20834,11 +20834,11 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P22" t="str">
         <f>CONCATENATE(".db #$", C22, B22, ", #%", IF(E22="R", "0", "1"),  DEC2BIN(D22-1,2), VLOOKUP(F22, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G22, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$56, #%11011100</v>
+        <v>.db #$56, #%11011010</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
@@ -20858,11 +20858,11 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P23" t="str">
         <f>CONCATENATE(".db #$", C23, B23, ", #%", IF(E23="R", "0", "1"),  DEC2BIN(D23-1,2), VLOOKUP(F23, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G23, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$27, #%10111100</v>
+        <v>.db #$27, #%10111010</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
@@ -20882,11 +20882,11 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P24" t="str">
         <f>CONCATENATE(".db #$", C24, B24, ", #%", IF(E24="R", "0", "1"),  DEC2BIN(D24-1,2), VLOOKUP(F24, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G24, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$67, #%11011100</v>
+        <v>.db #$67, #%11011010</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
@@ -20906,11 +20906,11 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P25" t="str">
         <f>CONCATENATE(".db #$", C25, B25, ", #%", IF(E25="R", "0", "1"),  DEC2BIN(D25-1,2), VLOOKUP(F25, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G25, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$38, #%00111100</v>
+        <v>.db #$38, #%00111010</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
@@ -20930,11 +20930,11 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P26" t="str">
         <f>CONCATENATE(".db #$", C26, B26, ", #%", IF(E26="R", "0", "1"),  DEC2BIN(D26-1,2), VLOOKUP(F26, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G26, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$78, #%10111100</v>
+        <v>.db #$78, #%10111010</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
@@ -20954,11 +20954,11 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P27" t="str">
         <f>CONCATENATE(".db #$", C27, B27, ", #%", IF(E27="R", "0", "1"),  DEC2BIN(D27-1,2), VLOOKUP(F27, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G27, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$09, #%00111100</v>
+        <v>.db #$09, #%00111010</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
@@ -20978,11 +20978,11 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P28" t="str">
         <f>CONCATENATE(".db #$", C28, B28, ", #%", IF(E28="R", "0", "1"),  DEC2BIN(D28-1,2), VLOOKUP(F28, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G28, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$39, #%00111100</v>
+        <v>.db #$39, #%00111010</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
@@ -21002,11 +21002,11 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P29" t="str">
         <f>CONCATENATE(".db #$", C29, B29, ", #%", IF(E29="R", "0", "1"),  DEC2BIN(D29-1,2), VLOOKUP(F29, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G29, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$89, #%00011100</v>
+        <v>.db #$89, #%00011010</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated level design sheet
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7745CDAD-3D77-4A3A-9743-16395CBAC4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07D23FE-588E-4181-B004-3E36EB34B67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="15936" windowHeight="10140" firstSheet="13" activeTab="25" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="11" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -5113,9 +5113,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF527098-673A-4A1B-8A76-8C4E7A5D0D04}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P54" sqref="P14:P54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P51" sqref="P51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6490,11 +6490,11 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P51" t="str">
         <f>CONCATENATE(".db #$", C51, B51, ", #%", IF(E51="R", "0", "1"),  DEC2BIN(D51-1,2), VLOOKUP(F51, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G51, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$96, #%01011100</v>
+        <v>.db #$96, #%01011010</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.3">
@@ -24437,7 +24437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA7A603-CC48-437E-96AE-32348CDF5D91}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="13" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P36" sqref="P36"/>
     </sheetView>

</xml_diff>

<commit_message>
Level design updates, block counter bug fix
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07D23FE-588E-4181-B004-3E36EB34B67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F7E052-480A-42DE-8979-80A816C1ACBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="11" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="15" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -322,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -1078,11 +1078,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="394">
+  <cellXfs count="395">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2213,6 +2228,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2561,10 +2579,10 @@
       <c r="B1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="392" t="s">
+      <c r="D1" s="393" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="393"/>
+      <c r="E1" s="394"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -5113,7 +5131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF527098-673A-4A1B-8A76-8C4E7A5D0D04}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="13" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P51" sqref="P51"/>
     </sheetView>
@@ -10783,9 +10801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E412488F-3473-4AB3-985F-ED3230803FB7}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10898,15 +10916,14 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="202" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="202" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="202" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="202" t="s">
+        <v>4</v>
+      </c>
       <c r="I3" s="5"/>
       <c r="J3" s="202" t="s">
         <v>4</v>
@@ -11298,7 +11315,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -11314,7 +11331,7 @@
       </c>
       <c r="P18" t="str">
         <f>CONCATENATE(".db #$", C18, B18, ", #%", IF(E18="R", "0", "1"),  DEC2BIN(D18-1,2), VLOOKUP(F18, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G18, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$31, #%00000100</v>
+        <v>.db #$41, #%00000100</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
@@ -11322,7 +11339,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -11338,7 +11355,7 @@
       </c>
       <c r="P19" t="str">
         <f>CONCATENATE(".db #$", C19, B19, ", #%", IF(E19="R", "0", "1"),  DEC2BIN(D19-1,2), VLOOKUP(F19, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G19, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$51, #%00000100</v>
+        <v>.db #$61, #%00000100</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
@@ -27744,8 +27761,8 @@
   <dimension ref="A1:R69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P32" sqref="P32"/>
+      <pane ySplit="13" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28153,11 +28170,11 @@
       <c r="F9" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>5</v>
+      <c r="G9" s="392" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>4</v>
       </c>
       <c r="I9" s="37" t="s">
         <v>4</v>
@@ -29345,7 +29362,7 @@
         <v>5</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" t="s">
         <v>17</v>
@@ -29358,7 +29375,7 @@
       </c>
       <c r="P57" t="str">
         <f>CONCATENATE(".db #$", C57, B57, ", #%", IF(E57="R", "0", "1"),  DEC2BIN(D57-1,2), VLOOKUP(F57, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G57, info!$K$5:$L$10, 2, FALSE))</f>
-        <v>.db #$57, #%00000001</v>
+        <v>.db #$57, #%00100001</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.3">
@@ -29651,6 +29668,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed level 18, prepared game over sequence
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F7E052-480A-42DE-8979-80A816C1ACBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7208396-E2D2-4671-8B7A-54B3B64F866F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="15" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="18" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -10801,7 +10801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E412488F-3473-4AB3-985F-ED3230803FB7}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
@@ -15088,9 +15088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF61D7D-E693-4D23-BB90-9B3E366E6A80}">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16413,11 +16413,11 @@
         <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P50" t="str">
         <f>CONCATENATE(".db #$", C50, B50, ", #%", IF(E50="R", "0", "1"),  DEC2BIN(D50-1,2), VLOOKUP(F50, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G50, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$88, #%10100011</v>
+        <v>.db #$88, #%10100000</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed animation and bonus looparound bugs
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB1F136-E5E6-4297-825C-76217B5628EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E5538E-E7AC-4396-9101-14D6E6F1E8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5193" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5194" uniqueCount="36">
   <si>
     <t>D</t>
   </si>
@@ -2243,14 +2243,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2592,10 +2592,10 @@
       <c r="B1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="394" t="s">
+      <c r="D1" s="395" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="395"/>
+      <c r="E1" s="396"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -16250,7 +16250,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="396" t="s">
+      <c r="N3" s="394" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="6"/>
@@ -16314,6 +16314,9 @@
       </c>
       <c r="I6" s="277" t="s">
         <v>6</v>
+      </c>
+      <c r="J6" s="129" t="s">
+        <v>4</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -16408,7 +16411,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="396" t="s">
+      <c r="N10" s="394" t="s">
         <v>5</v>
       </c>
       <c r="O10" s="6"/>
@@ -16463,20 +16466,20 @@
         <v>6</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="P14" t="str">
         <f>CONCATENATE(".db #$", C14, B14, ", #%", IF(E14="R", "0", "1"),  DEC2BIN(D14-1,2), VLOOKUP(F14, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G14, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$64, #%00100111</v>
+        <v>.db #$64, #%01000001</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -16484,7 +16487,7 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -16493,14 +16496,14 @@
         <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="P15" t="str">
         <f>CONCATENATE(".db #$", C15, B15, ", #%", IF(E15="R", "0", "1"),  DEC2BIN(D15-1,2), VLOOKUP(F15, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G15, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$64, #%00000001</v>
+        <v>.db #$74, #%00000111</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated level 11 and 15
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E5538E-E7AC-4396-9101-14D6E6F1E8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD03B2F-A3C7-4D0E-BD22-08E8DBC3E08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="16" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5194" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5188" uniqueCount="36">
   <si>
     <t>D</t>
   </si>
@@ -1104,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="397">
+  <cellXfs count="400">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1781,9 +1781,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2251,6 +2248,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2592,10 +2601,10 @@
       <c r="B1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="395" t="s">
+      <c r="D1" s="394" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="396"/>
+      <c r="E1" s="395"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -2607,7 +2616,7 @@
       </c>
       <c r="D2" s="87">
         <f>SUM(B:B)</f>
-        <v>1805</v>
+        <v>1801</v>
       </c>
       <c r="E2" s="88" t="s">
         <v>7</v>
@@ -2881,7 +2890,7 @@
       </c>
       <c r="B16">
         <f>'15'!Q$2</f>
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -4134,14 +4143,14 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="271" t="s">
+      <c r="J3" s="270" t="s">
         <v>4</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="278" t="s">
+      <c r="O3" s="277" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4152,7 +4161,7 @@
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="272" t="s">
+      <c r="E4" s="271" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="5"/>
@@ -4161,14 +4170,14 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="272" t="s">
+      <c r="L4" s="271" t="s">
         <v>4</v>
       </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="274" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" s="279" t="s">
+      <c r="N4" s="273" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="278" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4177,31 +4186,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="274" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="275" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="273" t="s">
+      <c r="C5" s="273" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="274" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="272" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="271" t="s">
+      <c r="G5" s="270" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="273" t="s">
+      <c r="L5" s="272" t="s">
         <v>4</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="246" t="s">
+      <c r="O5" s="245" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4212,7 +4221,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="273" t="s">
+      <c r="E6" s="272" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="5"/>
@@ -4221,7 +4230,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="273" t="s">
+      <c r="L6" s="272" t="s">
         <v>4</v>
       </c>
       <c r="M6" s="5"/>
@@ -4233,43 +4242,43 @@
         <v>5</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="274" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="276" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="276" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="275" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="274" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="276" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="276" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="275" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="274" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="276" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="276" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" s="275" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="280" t="s">
+      <c r="C7" s="273" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="275" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="275" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="274" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="273" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="275" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="275" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="274" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="273" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="275" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="275" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="274" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="279" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4327,7 +4336,7 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="281" t="s">
+      <c r="B10" s="280" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="5"/>
@@ -4351,7 +4360,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="5"/>
-      <c r="N10" s="273" t="s">
+      <c r="N10" s="272" t="s">
         <v>1</v>
       </c>
       <c r="O10" s="6"/>
@@ -4360,46 +4369,46 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="249" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="282" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="283" t="s">
+      <c r="B11" s="248" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="281" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="282" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="268" t="s">
+      <c r="F11" s="267" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="268" t="s">
+      <c r="H11" s="267" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="268" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="284" t="s">
-        <v>4</v>
-      </c>
-      <c r="L11" s="268" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" s="264" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="268" t="s">
-        <v>6</v>
-      </c>
-      <c r="O11" s="285" t="s">
+      <c r="J11" s="267" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="283" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="267" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="263" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="267" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="284" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6197,7 +6206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="13" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P51" sqref="P51"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14:P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6273,11 +6282,11 @@
       <c r="G2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="240" t="s">
+      <c r="H2" s="237" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="241" t="s">
+      <c r="J2" s="240" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="227" t="s">
@@ -6298,7 +6307,7 @@
       <c r="Q2">
         <v>83</v>
       </c>
-      <c r="R2" s="251" t="s">
+      <c r="R2" s="250" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6343,7 +6352,7 @@
       <c r="N3" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="242" t="s">
+      <c r="O3" s="241" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6360,13 +6369,13 @@
       <c r="D4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="E4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="36" t="s">
@@ -6388,7 +6397,7 @@
       <c r="N4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="243" t="s">
+      <c r="O4" s="242" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6396,7 +6405,7 @@
       <c r="A5" s="28">
         <v>3</v>
       </c>
-      <c r="B5" s="244" t="s">
+      <c r="B5" s="243" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="233" t="s">
@@ -6414,13 +6423,9 @@
       <c r="G5" s="234" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="46" t="s">
-        <v>4</v>
-      </c>
+      <c r="H5" s="396"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="141" t="s">
-        <v>4</v>
-      </c>
+      <c r="J5" s="396"/>
       <c r="K5" s="198" t="s">
         <v>4</v>
       </c>
@@ -6433,7 +6438,7 @@
       <c r="N5" s="233" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="245" t="s">
+      <c r="O5" s="244" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6450,23 +6455,23 @@
       <c r="D6" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="47" t="s">
+      <c r="E6" s="314" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="397" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="373" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="235" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="167" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="140" t="s">
+      <c r="J6" s="140" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="167" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="117" t="s">
@@ -6504,7 +6509,7 @@
       <c r="G7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="35" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="140" t="s">
@@ -6525,7 +6530,7 @@
       <c r="N7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="246" t="s">
+      <c r="O7" s="245" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6578,7 +6583,7 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="247" t="s">
+      <c r="B9" s="246" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5"/>
@@ -6593,7 +6598,7 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="248" t="s">
+      <c r="O9" s="247" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6601,7 +6606,7 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="247" t="s">
+      <c r="B10" s="246" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5"/>
@@ -6616,7 +6621,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="248" t="s">
+      <c r="O10" s="247" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6624,7 +6629,7 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="249" t="s">
+      <c r="B11" s="248" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="8"/>
@@ -6639,7 +6644,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="250" t="s">
+      <c r="O11" s="249" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7077,13 +7082,13 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>6</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -7096,18 +7101,18 @@
       </c>
       <c r="P31" t="str">
         <f>CONCATENATE(".db #$", C31, B31, ", #%", IF(E31="R", "0", "1"),  DEC2BIN(D31-1,2), VLOOKUP(F31, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G31, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$63, #%10100001</v>
+        <v>.db #$64, #%10000001</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <v>8</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -7120,7 +7125,7 @@
       </c>
       <c r="P32" t="str">
         <f>CONCATENATE(".db #$", C32, B32, ", #%", IF(E32="R", "0", "1"),  DEC2BIN(D32-1,2), VLOOKUP(F32, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G32, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$83, #%10100010</v>
+        <v>.db #$84, #%10000010</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
@@ -7720,19 +7725,19 @@
       <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="260" t="s">
+      <c r="B2" s="259" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="261" t="s">
+      <c r="G2" s="260" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="262" t="s">
+      <c r="J2" s="261" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="2"/>
@@ -7830,7 +7835,7 @@
       <c r="A6" s="28">
         <v>4</v>
       </c>
-      <c r="B6" s="263" t="s">
+      <c r="B6" s="262" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5"/>
@@ -7865,7 +7870,7 @@
       <c r="C7" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="259" t="s">
+      <c r="D7" s="258" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="5"/>
@@ -7980,20 +7985,20 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="264" t="s">
+      <c r="G11" s="263" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="265" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="266" t="s">
+      <c r="J11" s="264" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="265" t="s">
         <v>4</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="267" t="s">
+      <c r="N11" s="266" t="s">
         <v>4</v>
       </c>
       <c r="O11" s="222" t="s">
@@ -8598,38 +8603,38 @@
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="261" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="261" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="293" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="294" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="295" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="296" t="s">
+      <c r="C2" s="260" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="260" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="292" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="293" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="294" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="295" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="294" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="295" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="295" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="296" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="297" t="s">
+      <c r="J2" s="293" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="294" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="294" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="295" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="296" t="s">
         <v>4</v>
       </c>
       <c r="O2" s="209" t="s">
@@ -8653,7 +8658,7 @@
       <c r="D3" s="206" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="289" t="s">
+      <c r="E3" s="288" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="232" t="s">
@@ -8674,14 +8679,14 @@
       <c r="K3" s="233" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="259" t="s">
+      <c r="L3" s="258" t="s">
         <v>4</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="206" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="298" t="s">
+      <c r="O3" s="297" t="s">
         <v>4</v>
       </c>
     </row>
@@ -8700,29 +8705,29 @@
         <v>4</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="288" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="291" t="s">
+      <c r="G4" s="287" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="290" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="186" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="292" t="s">
+      <c r="J4" s="291" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="5"/>
-      <c r="L4" s="288" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="259" t="s">
+      <c r="L4" s="287" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="258" t="s">
         <v>4</v>
       </c>
       <c r="N4" s="206" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="298" t="s">
+      <c r="O4" s="297" t="s">
         <v>4</v>
       </c>
     </row>
@@ -8791,10 +8796,10 @@
       <c r="G6" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="290" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="290" t="s">
+      <c r="H6" s="289" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="289" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="43" t="s">
@@ -8803,16 +8808,16 @@
       <c r="K6" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="290" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" s="290" t="s">
+      <c r="L6" s="289" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="289" t="s">
         <v>1</v>
       </c>
       <c r="N6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="299" t="s">
+      <c r="O6" s="298" t="s">
         <v>1</v>
       </c>
     </row>
@@ -8839,7 +8844,7 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="300" t="s">
+      <c r="O7" s="299" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8878,7 +8883,7 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="263" t="s">
+      <c r="B9" s="262" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="5"/>
@@ -8899,7 +8904,7 @@
         <v>5</v>
       </c>
       <c r="N9" s="5"/>
-      <c r="O9" s="310" t="s">
+      <c r="O9" s="309" t="s">
         <v>35</v>
       </c>
     </row>
@@ -8957,7 +8962,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="301" t="s">
+      <c r="O11" s="300" t="s">
         <v>5</v>
       </c>
     </row>
@@ -10038,7 +10043,7 @@
       <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="302" t="s">
+      <c r="B2" s="301" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="239" t="s">
@@ -10047,37 +10052,37 @@
       <c r="D2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="303" t="s">
+      <c r="E2" s="302" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="303" t="s">
+      <c r="G2" s="302" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="303" t="s">
+      <c r="I2" s="302" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="303" t="s">
+      <c r="K2" s="302" t="s">
         <v>6</v>
       </c>
       <c r="L2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="303" t="s">
+      <c r="M2" s="302" t="s">
         <v>6</v>
       </c>
       <c r="N2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="304" t="s">
+      <c r="O2" s="303" t="s">
         <v>6</v>
       </c>
       <c r="Q2">
@@ -10091,7 +10096,7 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="306" t="s">
+      <c r="B3" s="305" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -10118,7 +10123,7 @@
         <v>6</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="307" t="s">
+      <c r="O3" s="306" t="s">
         <v>6</v>
       </c>
     </row>
@@ -10126,7 +10131,7 @@
       <c r="A4" s="28">
         <v>2</v>
       </c>
-      <c r="B4" s="308" t="s">
+      <c r="B4" s="307" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="5"/>
@@ -10172,7 +10177,7 @@
       <c r="B5" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="277" t="s">
+      <c r="C5" s="276" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="5"/>
@@ -10196,7 +10201,7 @@
         <v>6</v>
       </c>
       <c r="N5" s="5"/>
-      <c r="O5" s="277" t="s">
+      <c r="O5" s="276" t="s">
         <v>6</v>
       </c>
     </row>
@@ -10204,7 +10209,7 @@
       <c r="A6" s="28">
         <v>4</v>
       </c>
-      <c r="B6" s="247" t="s">
+      <c r="B6" s="246" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5"/>
@@ -10237,34 +10242,34 @@
       <c r="A7" s="28">
         <v>5</v>
       </c>
-      <c r="B7" s="309" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="277" t="s">
+      <c r="B7" s="308" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="276" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="277" t="s">
+      <c r="E7" s="276" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="277" t="s">
+      <c r="G7" s="276" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="277" t="s">
+      <c r="I7" s="276" t="s">
         <v>6</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="277" t="s">
+      <c r="K7" s="276" t="s">
         <v>6</v>
       </c>
       <c r="L7" s="5"/>
-      <c r="M7" s="277" t="s">
+      <c r="M7" s="276" t="s">
         <v>6</v>
       </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="277" t="s">
+      <c r="O7" s="276" t="s">
         <v>6</v>
       </c>
     </row>
@@ -10272,7 +10277,7 @@
       <c r="A8" s="28">
         <v>6</v>
       </c>
-      <c r="B8" s="308" t="s">
+      <c r="B8" s="307" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5"/>
@@ -10295,7 +10300,7 @@
       <c r="L8" s="189" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="287" t="s">
+      <c r="M8" s="286" t="s">
         <v>35</v>
       </c>
       <c r="N8" s="189" t="s">
@@ -10307,7 +10312,7 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="247" t="s">
+      <c r="B9" s="246" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="224" t="s">
@@ -10342,7 +10347,7 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="247" t="s">
+      <c r="B10" s="246" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5"/>
@@ -10385,30 +10390,30 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="249" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="268" t="s">
+      <c r="B11" s="248" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="267" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="305" t="s">
+      <c r="E11" s="304" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="305" t="s">
+      <c r="G11" s="304" t="s">
         <v>6</v>
       </c>
       <c r="H11" s="8"/>
-      <c r="I11" s="305" t="s">
+      <c r="I11" s="304" t="s">
         <v>6</v>
       </c>
       <c r="J11" s="8"/>
-      <c r="K11" s="305" t="s">
+      <c r="K11" s="304" t="s">
         <v>6</v>
       </c>
       <c r="L11" s="8"/>
-      <c r="M11" s="305" t="s">
+      <c r="M11" s="304" t="s">
         <v>6</v>
       </c>
       <c r="N11" s="8"/>
@@ -11863,11 +11868,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E412488F-3473-4AB3-985F-ED3230803FB7}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11925,7 +11930,7 @@
       <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="320" t="s">
+      <c r="B2" s="319" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="136" t="s">
@@ -11934,31 +11939,31 @@
       <c r="D2" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="135" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="321" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="135" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="321" t="s">
+      <c r="E2" s="320" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="398" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="399" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="398" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="320" t="s">
         <v>0</v>
       </c>
       <c r="N2" s="135" t="s">
@@ -11968,7 +11973,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="R2" t="s">
         <v>7</v>
@@ -11981,19 +11986,25 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="202" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="202" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="202" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="202" t="s">
+      <c r="F3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="M3" s="5"/>
@@ -12011,10 +12022,10 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="287" t="s">
+      <c r="I4" s="286" t="s">
         <v>35</v>
       </c>
+      <c r="J4" s="286"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -12102,7 +12113,7 @@
       <c r="N7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="O7" s="322" t="s">
+      <c r="O7" s="321" t="s">
         <v>4</v>
       </c>
     </row>
@@ -12192,7 +12203,7 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="323" t="s">
+      <c r="B10" s="322" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="44" t="s">
@@ -12201,7 +12212,7 @@
       <c r="D10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="290" t="s">
+      <c r="E10" s="289" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="43" t="s">
@@ -12210,10 +12221,10 @@
       <c r="G10" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="290" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="290" t="s">
+      <c r="H10" s="289" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="289" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="43" t="s">
@@ -12225,7 +12236,7 @@
       <c r="L10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="290" t="s">
+      <c r="M10" s="289" t="s">
         <v>4</v>
       </c>
       <c r="N10" s="18" t="s">
@@ -12382,7 +12393,7 @@
         <v>4</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
@@ -12395,7 +12406,7 @@
       </c>
       <c r="P18" t="str">
         <f>CONCATENATE(".db #$", C18, B18, ", #%", IF(E18="R", "0", "1"),  DEC2BIN(D18-1,2), VLOOKUP(F18, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G18, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$41, #%00000100</v>
+        <v>.db #$41, #%01100100</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
@@ -12403,10 +12414,10 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -12419,21 +12430,21 @@
       </c>
       <c r="P19" t="str">
         <f>CONCATENATE(".db #$", C19, B19, ", #%", IF(E19="R", "0", "1"),  DEC2BIN(D19-1,2), VLOOKUP(F19, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G19, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$61, #%00000100</v>
+        <v>.db #$81, #%01000100</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -12443,18 +12454,18 @@
       </c>
       <c r="P20" t="str">
         <f>CONCATENATE(".db #$", C20, B20, ", #%", IF(E20="R", "0", "1"),  DEC2BIN(D20-1,2), VLOOKUP(F20, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G20, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$81, #%00000100</v>
+        <v>.db #$05, #%11100100</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
         <v>17</v>
@@ -12467,7 +12478,7 @@
       </c>
       <c r="P21" t="str">
         <f>CONCATENATE(".db #$", C21, B21, ", #%", IF(E21="R", "0", "1"),  DEC2BIN(D21-1,2), VLOOKUP(F21, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G21, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$A1, #%00000100</v>
+        <v>.db #$15, #%01100100</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
@@ -12475,13 +12486,13 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F22" t="s">
         <v>4</v>
@@ -12491,7 +12502,7 @@
       </c>
       <c r="P22" t="str">
         <f>CONCATENATE(".db #$", C22, B22, ", #%", IF(E22="R", "0", "1"),  DEC2BIN(D22-1,2), VLOOKUP(F22, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G22, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$05, #%11100100</v>
+        <v>.db #$55, #%01100100</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
@@ -12499,7 +12510,7 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -12515,21 +12526,21 @@
       </c>
       <c r="P23" t="str">
         <f>CONCATENATE(".db #$", C23, B23, ", #%", IF(E23="R", "0", "1"),  DEC2BIN(D23-1,2), VLOOKUP(F23, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G23, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$15, #%01100100</v>
+        <v>.db #$95, #%01100100</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>5</v>
       </c>
-      <c r="C24">
-        <v>5</v>
+      <c r="C24" t="s">
+        <v>0</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>
@@ -12539,18 +12550,18 @@
       </c>
       <c r="P24" t="str">
         <f>CONCATENATE(".db #$", C24, B24, ", #%", IF(E24="R", "0", "1"),  DEC2BIN(D24-1,2), VLOOKUP(F24, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G24, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$55, #%01100100</v>
+        <v>.db #$D5, #%11100100</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
@@ -12563,21 +12574,21 @@
       </c>
       <c r="P25" t="str">
         <f>CONCATENATE(".db #$", C25, B25, ", #%", IF(E25="R", "0", "1"),  DEC2BIN(D25-1,2), VLOOKUP(F25, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G25, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$95, #%01100100</v>
+        <v>.db #$26, #%00000100</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
@@ -12587,7 +12598,7 @@
       </c>
       <c r="P26" t="str">
         <f>CONCATENATE(".db #$", C26, B26, ", #%", IF(E26="R", "0", "1"),  DEC2BIN(D26-1,2), VLOOKUP(F26, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G26, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$D5, #%11100100</v>
+        <v>.db #$46, #%01000100</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
@@ -12595,10 +12606,10 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
@@ -12611,18 +12622,18 @@
       </c>
       <c r="P27" t="str">
         <f>CONCATENATE(".db #$", C27, B27, ", #%", IF(E27="R", "0", "1"),  DEC2BIN(D27-1,2), VLOOKUP(F27, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G27, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$26, #%00000100</v>
+        <v>.db #$76, #%01100100</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>6</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>17</v>
@@ -12635,18 +12646,18 @@
       </c>
       <c r="P28" t="str">
         <f>CONCATENATE(".db #$", C28, B28, ", #%", IF(E28="R", "0", "1"),  DEC2BIN(D28-1,2), VLOOKUP(F28, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G28, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$46, #%01000100</v>
+        <v>.db #$C6, #%00000100</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
         <v>17</v>
@@ -12659,18 +12670,18 @@
       </c>
       <c r="P29" t="str">
         <f>CONCATENATE(".db #$", C29, B29, ", #%", IF(E29="R", "0", "1"),  DEC2BIN(D29-1,2), VLOOKUP(F29, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G29, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$76, #%01100100</v>
+        <v>.db #$17, #%00000100</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30">
-        <v>6</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
@@ -12683,7 +12694,7 @@
       </c>
       <c r="P30" t="str">
         <f>CONCATENATE(".db #$", C30, B30, ", #%", IF(E30="R", "0", "1"),  DEC2BIN(D30-1,2), VLOOKUP(F30, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G30, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$C6, #%00000100</v>
+        <v>.db #$37, #%01100100</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
@@ -12691,10 +12702,10 @@
         <v>7</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
         <v>17</v>
@@ -12707,18 +12718,18 @@
       </c>
       <c r="P31" t="str">
         <f>CONCATENATE(".db #$", C31, B31, ", #%", IF(E31="R", "0", "1"),  DEC2BIN(D31-1,2), VLOOKUP(F31, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G31, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$17, #%00000100</v>
+        <v>.db #$77, #%01000100</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>7</v>
       </c>
-      <c r="C32">
-        <v>3</v>
+      <c r="C32" t="s">
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
         <v>17</v>
@@ -12731,18 +12742,18 @@
       </c>
       <c r="P32" t="str">
         <f>CONCATENATE(".db #$", C32, B32, ", #%", IF(E32="R", "0", "1"),  DEC2BIN(D32-1,2), VLOOKUP(F32, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G32, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$37, #%01100100</v>
+        <v>.db #$B7, #%00000100</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
@@ -12755,18 +12766,18 @@
       </c>
       <c r="P33" t="str">
         <f>CONCATENATE(".db #$", C33, B33, ", #%", IF(E33="R", "0", "1"),  DEC2BIN(D33-1,2), VLOOKUP(F33, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G33, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$77, #%01000100</v>
+        <v>.db #$18, #%01100100</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
@@ -12779,7 +12790,7 @@
       </c>
       <c r="P34" t="str">
         <f>CONCATENATE(".db #$", C34, B34, ", #%", IF(E34="R", "0", "1"),  DEC2BIN(D34-1,2), VLOOKUP(F34, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G34, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$B7, #%00000100</v>
+        <v>.db #$58, #%01100100</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
@@ -12787,7 +12798,7 @@
         <v>8</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D35">
         <v>4</v>
@@ -12803,54 +12814,6 @@
       </c>
       <c r="P35" t="str">
         <f>CONCATENATE(".db #$", C35, B35, ", #%", IF(E35="R", "0", "1"),  DEC2BIN(D35-1,2), VLOOKUP(F35, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G35, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$18, #%01100100</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B36">
-        <v>8</v>
-      </c>
-      <c r="C36">
-        <v>5</v>
-      </c>
-      <c r="D36">
-        <v>4</v>
-      </c>
-      <c r="E36" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" t="s">
-        <v>4</v>
-      </c>
-      <c r="G36" t="s">
-        <v>26</v>
-      </c>
-      <c r="P36" t="str">
-        <f>CONCATENATE(".db #$", C36, B36, ", #%", IF(E36="R", "0", "1"),  DEC2BIN(D36-1,2), VLOOKUP(F36, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G36, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$58, #%01100100</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B37">
-        <v>8</v>
-      </c>
-      <c r="C37">
-        <v>9</v>
-      </c>
-      <c r="D37">
-        <v>4</v>
-      </c>
-      <c r="E37" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37" t="s">
-        <v>26</v>
-      </c>
-      <c r="P37" t="str">
-        <f>CONCATENATE(".db #$", C37, B37, ", #%", IF(E37="R", "0", "1"),  DEC2BIN(D37-1,2), VLOOKUP(F37, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G37, info!$K$5:$L$11, 2, FALSE))</f>
         <v>.db #$98, #%01100100</v>
       </c>
     </row>
@@ -12927,7 +12890,7 @@
       <c r="C2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="269" t="s">
+      <c r="D2" s="268" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="55" t="s">
@@ -12954,13 +12917,13 @@
       <c r="L2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="317" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="317" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="318" t="s">
+      <c r="M2" s="316" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="316" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="317" t="s">
         <v>4</v>
       </c>
       <c r="Q2">
@@ -13044,7 +13007,7 @@
       <c r="J4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="314" t="s">
+      <c r="K4" s="313" t="s">
         <v>4</v>
       </c>
       <c r="L4" s="46" t="s">
@@ -13089,7 +13052,7 @@
       <c r="J5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="315" t="s">
+      <c r="K5" s="314" t="s">
         <v>4</v>
       </c>
       <c r="L5" s="42" t="s">
@@ -13281,7 +13244,7 @@
       <c r="N9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="307" t="s">
+      <c r="O9" s="306" t="s">
         <v>6</v>
       </c>
     </row>
@@ -13302,7 +13265,7 @@
       <c r="F10" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="312" t="s">
+      <c r="G10" s="311" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="49" t="s">
@@ -13326,7 +13289,7 @@
       <c r="N10" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="O10" s="319" t="s">
+      <c r="O10" s="318" t="s">
         <v>1</v>
       </c>
     </row>
@@ -13339,7 +13302,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="284" t="s">
+      <c r="G11" s="283" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="8"/>
@@ -13349,7 +13312,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="311" t="s">
+      <c r="O11" s="310" t="s">
         <v>35</v>
       </c>
     </row>
@@ -14470,7 +14433,7 @@
       <c r="G2" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="321" t="s">
+      <c r="H2" s="320" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="139" t="s">
@@ -14485,7 +14448,7 @@
       <c r="L2" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="321" t="s">
+      <c r="M2" s="320" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="2"/>
@@ -14510,23 +14473,23 @@
       <c r="D3" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="313" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="313" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="313" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="324" t="s">
+      <c r="E3" s="312" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="312" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="312" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="323" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="324" t="s">
+      <c r="K3" s="323" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="140" t="s">
@@ -14536,7 +14499,7 @@
       <c r="N3" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="325" t="s">
+      <c r="O3" s="324" t="s">
         <v>5</v>
       </c>
     </row>
@@ -14553,7 +14516,7 @@
       <c r="D4" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="324" t="s">
+      <c r="E4" s="323" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="117" t="s">
@@ -14581,7 +14544,7 @@
       <c r="N4" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="326" t="s">
+      <c r="O4" s="325" t="s">
         <v>4</v>
       </c>
     </row>
@@ -14605,7 +14568,7 @@
       <c r="G5" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="354" t="s">
+      <c r="H5" s="353" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="140" t="s">
@@ -14626,7 +14589,7 @@
       <c r="N5" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="327" t="s">
+      <c r="O5" s="326" t="s">
         <v>4</v>
       </c>
     </row>
@@ -14634,7 +14597,7 @@
       <c r="A6" s="28">
         <v>4</v>
       </c>
-      <c r="B6" s="328" t="s">
+      <c r="B6" s="327" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="141" t="s">
@@ -14671,7 +14634,7 @@
       <c r="N6" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="327" t="s">
+      <c r="O6" s="326" t="s">
         <v>4</v>
       </c>
     </row>
@@ -14716,7 +14679,7 @@
       <c r="N7" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="329" t="s">
+      <c r="O7" s="328" t="s">
         <v>4</v>
       </c>
     </row>
@@ -14774,7 +14737,7 @@
       <c r="D9" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="324" t="s">
+      <c r="E9" s="323" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="165" t="s">
@@ -14789,16 +14752,16 @@
       <c r="I9" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="324" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" s="316" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" s="313" t="s">
-        <v>4</v>
-      </c>
-      <c r="M9" s="324" t="s">
+      <c r="J9" s="323" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="315" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="312" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="323" t="s">
         <v>5</v>
       </c>
       <c r="N9" s="5"/>
@@ -14824,10 +14787,10 @@
         <v>4</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="316" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="313" t="s">
+      <c r="H10" s="315" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="312" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="117" t="s">
@@ -14842,10 +14805,10 @@
       <c r="M10" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="313" t="s">
-        <v>5</v>
-      </c>
-      <c r="O10" s="325" t="s">
+      <c r="N10" s="312" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="324" t="s">
         <v>4</v>
       </c>
     </row>
@@ -14853,7 +14816,7 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="330" t="s">
+      <c r="B11" s="329" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="182" t="s">
@@ -14872,7 +14835,7 @@
       <c r="H11" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="331" t="s">
+      <c r="I11" s="330" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="181" t="s">
@@ -14887,10 +14850,10 @@
       <c r="M11" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="331" t="s">
-        <v>4</v>
-      </c>
-      <c r="O11" s="332" t="s">
+      <c r="N11" s="330" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="331" t="s">
         <v>4</v>
       </c>
     </row>
@@ -16152,8 +16115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA56FFEF-F7C8-4860-BE54-456CF04E33C0}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14:P21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16250,7 +16213,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="394" t="s">
+      <c r="N3" s="393" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="6"/>
@@ -16268,7 +16231,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="393" t="s">
+      <c r="K4" s="392" t="s">
         <v>35</v>
       </c>
       <c r="L4" s="5"/>
@@ -16312,7 +16275,7 @@
       <c r="H6" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="277" t="s">
+      <c r="I6" s="276" t="s">
         <v>6</v>
       </c>
       <c r="J6" s="129" t="s">
@@ -16411,7 +16374,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="394" t="s">
+      <c r="N10" s="393" t="s">
         <v>5</v>
       </c>
       <c r="O10" s="6"/>
@@ -16722,27 +16685,27 @@
       <c r="B2" s="219" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="270"/>
+      <c r="C2" s="269"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="338" t="s">
+      <c r="G2" s="337" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="262" t="s">
+      <c r="J2" s="261" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="339" t="s">
+      <c r="O2" s="338" t="s">
         <v>1</v>
       </c>
       <c r="Q2">
@@ -16756,7 +16719,7 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="340" t="s">
+      <c r="B3" s="339" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5"/>
@@ -16769,7 +16732,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="287" t="s">
+      <c r="M3" s="286" t="s">
         <v>35</v>
       </c>
       <c r="N3" s="5"/>
@@ -16872,7 +16835,7 @@
       <c r="A7" s="28">
         <v>5</v>
       </c>
-      <c r="B7" s="308" t="s">
+      <c r="B7" s="307" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5"/>
@@ -16901,40 +16864,40 @@
       <c r="A8" s="28">
         <v>6</v>
       </c>
-      <c r="B8" s="247" t="s">
+      <c r="B8" s="246" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="81" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="334" t="s">
+      <c r="E8" s="333" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="335" t="s">
+      <c r="G8" s="334" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="31" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="J8" s="334" t="s">
+      <c r="J8" s="333" t="s">
         <v>6</v>
       </c>
       <c r="K8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="335" t="s">
+      <c r="L8" s="334" t="s">
         <v>6</v>
       </c>
       <c r="M8" s="31" t="s">
         <v>6</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="341" t="s">
+      <c r="O8" s="340" t="s">
         <v>6</v>
       </c>
     </row>
@@ -16942,7 +16905,7 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="342" t="s">
+      <c r="B9" s="341" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="224" t="s">
@@ -16954,13 +16917,13 @@
       <c r="E9" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="335" t="s">
+      <c r="F9" s="334" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="203" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="335" t="s">
+      <c r="H9" s="334" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="232" t="s">
@@ -16969,19 +16932,19 @@
       <c r="J9" s="234" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="335" t="s">
+      <c r="K9" s="334" t="s">
         <v>6</v>
       </c>
       <c r="L9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="M9" s="335" t="s">
+      <c r="M9" s="334" t="s">
         <v>6</v>
       </c>
       <c r="N9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="243" t="s">
+      <c r="O9" s="242" t="s">
         <v>4</v>
       </c>
     </row>
@@ -16989,16 +16952,16 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="343" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="336" t="s">
+      <c r="B10" s="342" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="335" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="252" t="s">
+      <c r="E10" s="251" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="224" t="s">
@@ -17007,7 +16970,7 @@
       <c r="G10" s="204" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="336" t="s">
+      <c r="H10" s="335" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="186" t="s">
@@ -17022,13 +16985,13 @@
       <c r="L10" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="336" t="s">
+      <c r="M10" s="335" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="189" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="344" t="s">
+      <c r="O10" s="343" t="s">
         <v>4</v>
       </c>
     </row>
@@ -17036,46 +16999,46 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="345" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="346" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="347" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="348" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="268" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="265" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="349" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="266" t="s">
+      <c r="B11" s="344" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="345" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="346" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="347" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="267" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="264" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="348" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="265" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="218" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="268" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="350" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" s="351" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="352" t="s">
-        <v>4</v>
-      </c>
-      <c r="O11" s="353" t="s">
+      <c r="K11" s="267" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="349" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="350" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="351" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="352" t="s">
         <v>4</v>
       </c>
     </row>
@@ -18223,20 +18186,20 @@
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="288" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="259" t="s">
+      <c r="J3" s="287" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="258" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="5"/>
-      <c r="M3" s="288" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="291" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="245" t="s">
+      <c r="M3" s="287" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="290" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="244" t="s">
         <v>5</v>
       </c>
     </row>
@@ -18285,7 +18248,7 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="288" t="s">
+      <c r="D5" s="287" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="234" t="s">
@@ -18295,7 +18258,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="288" t="s">
+      <c r="J5" s="287" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="234" t="s">
@@ -18305,7 +18268,7 @@
       <c r="M5" s="232" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="259" t="s">
+      <c r="N5" s="258" t="s">
         <v>5</v>
       </c>
       <c r="O5" s="6"/>
@@ -18314,7 +18277,7 @@
       <c r="A6" s="28">
         <v>4</v>
       </c>
-      <c r="B6" s="355" t="s">
+      <c r="B6" s="354" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5"/>
@@ -18380,7 +18343,7 @@
       <c r="N7" s="204" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="298" t="s">
+      <c r="O7" s="297" t="s">
         <v>5</v>
       </c>
     </row>
@@ -18388,7 +18351,7 @@
       <c r="A8" s="28">
         <v>6</v>
       </c>
-      <c r="B8" s="356" t="s">
+      <c r="B8" s="355" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="5"/>
@@ -18415,7 +18378,7 @@
         <v>5</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="298" t="s">
+      <c r="O8" s="297" t="s">
         <v>5</v>
       </c>
     </row>
@@ -18423,7 +18386,7 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="357" t="s">
+      <c r="B9" s="356" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="5"/>
@@ -18485,7 +18448,7 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="358" t="s">
+      <c r="B11" s="357" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="78" t="s">
@@ -19365,46 +19328,46 @@
       <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="360" t="s">
+      <c r="B2" s="359" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="295" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="296" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="365" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="295" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="296" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="269" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="294" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="295" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="297" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="269" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="293" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="361" t="s">
+      <c r="D2" s="294" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="295" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="364" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="294" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="295" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="293" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="294" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="296" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="292" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="360" t="s">
         <v>4</v>
       </c>
       <c r="Q2">
@@ -19418,7 +19381,7 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="244" t="s">
+      <c r="B3" s="243" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="233" t="s">
@@ -19447,7 +19410,7 @@
       <c r="N3" s="234" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="325" t="s">
+      <c r="O3" s="324" t="s">
         <v>0</v>
       </c>
     </row>
@@ -19481,10 +19444,10 @@
       <c r="F5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="335" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="335" t="s">
+      <c r="G5" s="334" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="334" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="31" t="s">
@@ -19493,10 +19456,10 @@
       <c r="J5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="335" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="359" t="s">
+      <c r="K5" s="334" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="358" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="5"/>
@@ -19511,7 +19474,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="333" t="s">
+      <c r="F6" s="332" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="94" t="s">
@@ -19525,7 +19488,7 @@
       <c r="K6" s="198" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="359" t="s">
+      <c r="L6" s="358" t="s">
         <v>6</v>
       </c>
       <c r="M6" s="5"/>
@@ -19551,7 +19514,7 @@
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="366" t="s">
+      <c r="K7" s="365" t="s">
         <v>35</v>
       </c>
       <c r="L7" s="36" t="s">
@@ -19598,7 +19561,7 @@
         <v>6</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="307" t="s">
+      <c r="O8" s="306" t="s">
         <v>6</v>
       </c>
     </row>
@@ -19627,7 +19590,7 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="244" t="s">
+      <c r="B10" s="243" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="30" t="s">
@@ -19666,7 +19629,7 @@
       <c r="N10" s="234" t="s">
         <v>4</v>
       </c>
-      <c r="O10" s="325" t="s">
+      <c r="O10" s="324" t="s">
         <v>0</v>
       </c>
     </row>
@@ -19674,46 +19637,46 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="362" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="363" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="349" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="266" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="305" t="s">
+      <c r="B11" s="361" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="362" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="348" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="265" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="304" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="265" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="349" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="349" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="266" t="s">
-        <v>4</v>
-      </c>
-      <c r="L11" s="265" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" s="349" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="349" t="s">
-        <v>4</v>
-      </c>
-      <c r="O11" s="364" t="s">
+      <c r="H11" s="264" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="348" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="348" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="265" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="264" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="348" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="348" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="363" t="s">
         <v>4</v>
       </c>
     </row>
@@ -20698,13 +20661,13 @@
       <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="368" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="338" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="369" t="s">
+      <c r="B2" s="367" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="337" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="368" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="239" t="s">
@@ -20713,10 +20676,10 @@
       <c r="F2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="370" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="369" t="s">
+      <c r="G2" s="369" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="368" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="239" t="s">
@@ -20725,19 +20688,19 @@
       <c r="J2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="370" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="369" t="s">
+      <c r="K2" s="369" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="368" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="239" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="370" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="371" t="s">
+      <c r="N2" s="369" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="370" t="s">
         <v>1</v>
       </c>
       <c r="Q2">
@@ -20803,7 +20766,7 @@
       <c r="N4" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="242" t="s">
+      <c r="O4" s="241" t="s">
         <v>4</v>
       </c>
     </row>
@@ -20814,7 +20777,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="367" t="s">
+      <c r="E5" s="366" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="117" t="s">
@@ -20885,7 +20848,7 @@
       <c r="N6" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="242" t="s">
+      <c r="O6" s="241" t="s">
         <v>4</v>
       </c>
     </row>
@@ -20948,7 +20911,7 @@
       <c r="M8" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="252" t="s">
+      <c r="N8" s="251" t="s">
         <v>4</v>
       </c>
       <c r="O8" s="6"/>
@@ -20957,7 +20920,7 @@
       <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="328" t="s">
+      <c r="B9" s="327" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="118" t="s">
@@ -20993,7 +20956,7 @@
       <c r="M9" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="N9" s="253" t="s">
+      <c r="N9" s="252" t="s">
         <v>4</v>
       </c>
       <c r="O9" s="6"/>
@@ -21002,7 +20965,7 @@
       <c r="A10" s="28">
         <v>8</v>
       </c>
-      <c r="B10" s="281" t="s">
+      <c r="B10" s="280" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="199" t="s">
@@ -21038,7 +21001,7 @@
       <c r="M10" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="254" t="s">
+      <c r="N10" s="253" t="s">
         <v>4</v>
       </c>
       <c r="O10" s="6"/>
@@ -21047,7 +21010,7 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="372" t="s">
+      <c r="B11" s="371" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="8"/>
@@ -21877,7 +21840,7 @@
       <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="320" t="s">
+      <c r="B2" s="319" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="136" t="s">
@@ -21886,7 +21849,7 @@
       <c r="D2" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="321" t="s">
+      <c r="E2" s="320" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="135" t="s">
@@ -21898,7 +21861,7 @@
       <c r="H2" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="321" t="s">
+      <c r="I2" s="320" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="135" t="s">
@@ -21910,7 +21873,7 @@
       <c r="L2" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="321" t="s">
+      <c r="M2" s="320" t="s">
         <v>0</v>
       </c>
       <c r="N2" s="135" t="s">
@@ -21989,7 +21952,7 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="277" t="s">
+      <c r="M5" s="276" t="s">
         <v>6</v>
       </c>
       <c r="N5" s="5"/>
@@ -22010,14 +21973,14 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="373" t="s">
+      <c r="I6" s="372" t="s">
         <v>35</v>
       </c>
       <c r="J6" s="82" t="s">
         <v>6</v>
       </c>
       <c r="K6" s="5"/>
-      <c r="L6" s="277" t="s">
+      <c r="L6" s="276" t="s">
         <v>6</v>
       </c>
       <c r="M6" s="5"/>
@@ -22136,7 +22099,7 @@
         <v>4</v>
       </c>
       <c r="N10" s="5"/>
-      <c r="O10" s="319" t="s">
+      <c r="O10" s="318" t="s">
         <v>4</v>
       </c>
     </row>
@@ -22780,46 +22743,46 @@
       <c r="A2" s="28">
         <v>0</v>
       </c>
-      <c r="B2" s="380" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="317" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="317" t="s">
+      <c r="B2" s="379" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="316" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="316" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="338" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="255" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="257" t="s">
+      <c r="F2" s="337" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="254" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="256" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="381" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="255" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="382" t="s">
+      <c r="K2" s="380" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="254" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="381" t="s">
         <v>4</v>
       </c>
       <c r="Q2">
@@ -22860,7 +22823,7 @@
       <c r="J3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="253" t="s">
+      <c r="K3" s="252" t="s">
         <v>4</v>
       </c>
       <c r="L3" s="199" t="s">
@@ -22872,7 +22835,7 @@
       <c r="N3" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="242" t="s">
+      <c r="O3" s="241" t="s">
         <v>4</v>
       </c>
     </row>
@@ -22907,7 +22870,7 @@
       <c r="J4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="253" t="s">
+      <c r="K4" s="252" t="s">
         <v>4</v>
       </c>
       <c r="L4" s="29" t="s">
@@ -22919,7 +22882,7 @@
       <c r="N4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="246" t="s">
+      <c r="O4" s="245" t="s">
         <v>6</v>
       </c>
     </row>
@@ -22936,7 +22899,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="253" t="s">
+      <c r="K5" s="252" t="s">
         <v>4</v>
       </c>
       <c r="L5" s="5"/>
@@ -22969,13 +22932,13 @@
       <c r="H6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="252" t="s">
+      <c r="I6" s="251" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="252" t="s">
+      <c r="K6" s="251" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="81" t="s">
@@ -22993,34 +22956,34 @@
       <c r="A7" s="28">
         <v>5</v>
       </c>
-      <c r="B7" s="383" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="337" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="337" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="377" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="367" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="337" t="s">
+      <c r="B7" s="382" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="336" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="336" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="376" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="366" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="336" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="253" t="s">
+      <c r="I7" s="252" t="s">
         <v>4</v>
       </c>
       <c r="J7" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="253" t="s">
+      <c r="K7" s="252" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="82" t="s">
@@ -23049,19 +23012,19 @@
       <c r="F8" s="235" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="377" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="374" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="253" t="s">
+      <c r="G8" s="376" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="373" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="252" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="253" t="s">
+      <c r="K8" s="252" t="s">
         <v>4</v>
       </c>
       <c r="L8" s="36" t="s">
@@ -23069,7 +23032,7 @@
       </c>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="307" t="s">
+      <c r="O8" s="306" t="s">
         <v>6</v>
       </c>
     </row>
@@ -23081,28 +23044,28 @@
       <c r="C9" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="378" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="378" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="379" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="253" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="375" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="253" t="s">
+      <c r="D9" s="377" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="377" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="378" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="252" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="374" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="252" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="253" t="s">
+      <c r="K9" s="252" t="s">
         <v>4</v>
       </c>
       <c r="L9" s="81" t="s">
@@ -23112,7 +23075,7 @@
       <c r="N9" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="384" t="s">
+      <c r="O9" s="383" t="s">
         <v>1</v>
       </c>
     </row>
@@ -23133,10 +23096,10 @@
       <c r="F10" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="253" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="376" t="s">
+      <c r="G10" s="252" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="375" t="s">
         <v>1</v>
       </c>
       <c r="I10" s="199" t="s">
@@ -23155,7 +23118,7 @@
       <c r="N10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="385" t="s">
+      <c r="O10" s="384" t="s">
         <v>1</v>
       </c>
     </row>
@@ -23167,35 +23130,35 @@
       <c r="C11" s="221" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="346" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="346" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="347" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="348" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="386" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="387" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="346" t="s">
-        <v>4</v>
-      </c>
-      <c r="K11" s="347" t="s">
-        <v>4</v>
-      </c>
-      <c r="L11" s="305" t="s">
+      <c r="D11" s="345" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="345" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="346" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="347" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="385" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="386" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="345" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="346" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="304" t="s">
         <v>6</v>
       </c>
       <c r="M11" s="8"/>
-      <c r="N11" s="388" t="s">
+      <c r="N11" s="387" t="s">
         <v>35</v>
       </c>
       <c r="O11" s="9"/>
@@ -24189,7 +24152,7 @@
       <c r="E2" s="227" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="258" t="s">
+      <c r="F2" s="257" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="2"/>
@@ -24197,7 +24160,7 @@
       <c r="I2" s="227" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="269" t="s">
+      <c r="J2" s="268" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="2"/>
@@ -24296,7 +24259,7 @@
       <c r="E5" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="287" t="s">
+      <c r="F5" s="286" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="5"/>
@@ -24482,7 +24445,7 @@
       <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="286" t="s">
+      <c r="B11" s="285" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="160" t="s">
@@ -25413,32 +25376,32 @@
       <c r="B2" s="219" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="255" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="257" t="s">
+      <c r="C2" s="254" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="256" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="255" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="257" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="303" t="s">
+      <c r="H2" s="254" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="256" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="302" t="s">
         <v>6</v>
       </c>
       <c r="M2" s="2"/>
@@ -25455,7 +25418,7 @@
       <c r="A3" s="28">
         <v>1</v>
       </c>
-      <c r="B3" s="389" t="s">
+      <c r="B3" s="388" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5"/>
@@ -25465,7 +25428,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="391" t="s">
+      <c r="J3" s="390" t="s">
         <v>35</v>
       </c>
       <c r="K3" s="5"/>
@@ -25492,7 +25455,7 @@
       <c r="E4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="277" t="s">
+      <c r="F4" s="276" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="5"/>
@@ -25607,7 +25570,7 @@
       <c r="N8" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="246" t="s">
+      <c r="O8" s="245" t="s">
         <v>6</v>
       </c>
     </row>
@@ -25672,10 +25635,10 @@
       <c r="B11" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="331" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="331" t="s">
+      <c r="C11" s="330" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="330" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="181" t="s">
@@ -25684,10 +25647,10 @@
       <c r="F11" s="182" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="331" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="331" t="s">
+      <c r="G11" s="330" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="330" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="181" t="s">
@@ -25699,16 +25662,16 @@
       <c r="K11" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="390" t="s">
+      <c r="L11" s="389" t="s">
         <v>6</v>
       </c>
       <c r="M11" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="N11" s="331" t="s">
-        <v>4</v>
-      </c>
-      <c r="O11" s="332" t="s">
+      <c r="N11" s="330" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="331" t="s">
         <v>4</v>
       </c>
     </row>
@@ -29741,7 +29704,7 @@
       <c r="F9" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="392" t="s">
+      <c r="G9" s="391" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="50" t="s">
@@ -32446,13 +32409,13 @@
         <v>4</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="255" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="256" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="257" t="s">
+      <c r="H2" s="254" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="256" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="2"/>
@@ -32488,7 +32451,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="5"/>
-      <c r="I3" s="252" t="s">
+      <c r="I3" s="251" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="5"/>
@@ -32523,7 +32486,7 @@
       <c r="H4" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="253" t="s">
+      <c r="I4" s="252" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="158" t="s">
@@ -32556,7 +32519,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="254" t="s">
+      <c r="I5" s="253" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="5"/>
@@ -32624,7 +32587,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="252" t="s">
+      <c r="I7" s="251" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="5"/>
@@ -32659,7 +32622,7 @@
       <c r="H8" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="253" t="s">
+      <c r="I8" s="252" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="158" t="s">
@@ -32692,7 +32655,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="254" t="s">
+      <c r="I9" s="253" t="s">
         <v>5</v>
       </c>
       <c r="J9" s="5"/>

</xml_diff>

<commit_message>
Updated level 12 and 15, finetuned nudge and speed
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD03B2F-A3C7-4D0E-BD22-08E8DBC3E08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85CB5AC-A951-4271-8B95-ADDE65803736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="16" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="13" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5188" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5182" uniqueCount="36">
   <si>
     <t>D</t>
   </si>
@@ -1104,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="400">
+  <cellXfs count="401">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2243,6 +2243,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2252,13 +2255,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2601,10 +2602,10 @@
       <c r="B1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="394" t="s">
+      <c r="D1" s="395" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="395"/>
+      <c r="E1" s="396"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -2616,7 +2617,7 @@
       </c>
       <c r="D2" s="87">
         <f>SUM(B:B)</f>
-        <v>1801</v>
+        <v>1799</v>
       </c>
       <c r="E2" s="88" t="s">
         <v>7</v>
@@ -2890,7 +2891,7 @@
       </c>
       <c r="B16">
         <f>'15'!Q$2</f>
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -6423,9 +6424,9 @@
       <c r="G5" s="234" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="396"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="396"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="198" t="s">
         <v>4</v>
       </c>
@@ -6458,7 +6459,7 @@
       <c r="E6" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="397" t="s">
+      <c r="F6" s="394" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="373" t="s">
@@ -7665,7 +7666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D6449E-BDD8-47F1-8C6B-F5B8184718A5}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P34" sqref="P14:P34"/>
     </sheetView>
@@ -11868,11 +11869,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E412488F-3473-4AB3-985F-ED3230803FB7}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14:P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11942,25 +11943,25 @@
       <c r="E2" s="320" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="398" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="399" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="398" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="268" t="s">
+      <c r="F2" s="135" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="136" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="136" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="320" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="135" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="136" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="136" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="320" t="s">
@@ -11973,7 +11974,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R2" t="s">
         <v>7</v>
@@ -11984,31 +11985,26 @@
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="C3" s="398"/>
+      <c r="D3" s="399"/>
+      <c r="E3" s="398"/>
+      <c r="F3" s="397"/>
+      <c r="G3" s="397"/>
+      <c r="H3" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="289" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="289" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="397"/>
+      <c r="M3" s="398"/>
+      <c r="N3" s="398"/>
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12016,20 +12012,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="286" t="s">
+      <c r="C4" s="398"/>
+      <c r="D4" s="398"/>
+      <c r="E4" s="398"/>
+      <c r="F4" s="398"/>
+      <c r="G4" s="398"/>
+      <c r="H4" s="398"/>
+      <c r="I4" s="400" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="286"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="J4" s="400"/>
+      <c r="K4" s="398"/>
+      <c r="L4" s="398"/>
+      <c r="M4" s="398"/>
+      <c r="N4" s="398"/>
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12037,18 +12033,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="C5" s="398"/>
+      <c r="D5" s="398"/>
+      <c r="E5" s="398"/>
+      <c r="F5" s="398"/>
+      <c r="G5" s="398"/>
+      <c r="H5" s="398"/>
+      <c r="I5" s="398"/>
+      <c r="J5" s="398"/>
+      <c r="K5" s="398"/>
+      <c r="L5" s="398"/>
+      <c r="M5" s="398"/>
+      <c r="N5" s="398"/>
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12056,18 +12052,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="C6" s="398"/>
+      <c r="D6" s="398"/>
+      <c r="E6" s="398"/>
+      <c r="F6" s="398"/>
+      <c r="G6" s="398"/>
+      <c r="H6" s="398"/>
+      <c r="I6" s="398"/>
+      <c r="J6" s="398"/>
+      <c r="K6" s="398"/>
+      <c r="L6" s="398"/>
+      <c r="M6" s="398"/>
+      <c r="N6" s="398"/>
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12124,11 +12120,11 @@
       <c r="B8" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="398"/>
       <c r="D8" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="398"/>
       <c r="F8" s="16" t="s">
         <v>4</v>
       </c>
@@ -12150,7 +12146,7 @@
       <c r="L8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="5"/>
+      <c r="M8" s="398"/>
       <c r="N8" s="202" t="s">
         <v>4</v>
       </c>
@@ -12168,7 +12164,7 @@
       <c r="C9" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="398"/>
       <c r="E9" s="16" t="s">
         <v>4</v>
       </c>
@@ -12190,11 +12186,11 @@
       <c r="K9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="398"/>
       <c r="M9" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="5"/>
+      <c r="N9" s="398"/>
       <c r="O9" s="210" t="s">
         <v>4</v>
       </c>
@@ -12390,7 +12386,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -12406,21 +12402,21 @@
       </c>
       <c r="P18" t="str">
         <f>CONCATENATE(".db #$", C18, B18, ", #%", IF(E18="R", "0", "1"),  DEC2BIN(D18-1,2), VLOOKUP(F18, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G18, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$41, #%01100100</v>
+        <v>.db #$61, #%01100100</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
         <v>4</v>
@@ -12430,7 +12426,7 @@
       </c>
       <c r="P19" t="str">
         <f>CONCATENATE(".db #$", C19, B19, ", #%", IF(E19="R", "0", "1"),  DEC2BIN(D19-1,2), VLOOKUP(F19, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G19, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$81, #%01000100</v>
+        <v>.db #$05, #%11100100</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
@@ -12438,13 +12434,13 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -12454,7 +12450,7 @@
       </c>
       <c r="P20" t="str">
         <f>CONCATENATE(".db #$", C20, B20, ", #%", IF(E20="R", "0", "1"),  DEC2BIN(D20-1,2), VLOOKUP(F20, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G20, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$05, #%11100100</v>
+        <v>.db #$15, #%01100100</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
@@ -12462,7 +12458,7 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -12478,7 +12474,7 @@
       </c>
       <c r="P21" t="str">
         <f>CONCATENATE(".db #$", C21, B21, ", #%", IF(E21="R", "0", "1"),  DEC2BIN(D21-1,2), VLOOKUP(F21, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G21, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$15, #%01100100</v>
+        <v>.db #$55, #%01100100</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
@@ -12486,7 +12482,7 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -12502,21 +12498,21 @@
       </c>
       <c r="P22" t="str">
         <f>CONCATENATE(".db #$", C22, B22, ", #%", IF(E22="R", "0", "1"),  DEC2BIN(D22-1,2), VLOOKUP(F22, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G22, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$55, #%01100100</v>
+        <v>.db #$95, #%01100100</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>5</v>
       </c>
-      <c r="C23">
-        <v>9</v>
+      <c r="C23" t="s">
+        <v>0</v>
       </c>
       <c r="D23">
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
@@ -12526,21 +12522,21 @@
       </c>
       <c r="P23" t="str">
         <f>CONCATENATE(".db #$", C23, B23, ", #%", IF(E23="R", "0", "1"),  DEC2BIN(D23-1,2), VLOOKUP(F23, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G23, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$95, #%01100100</v>
+        <v>.db #$D5, #%11100100</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F24" t="s">
         <v>4</v>
@@ -12550,7 +12546,7 @@
       </c>
       <c r="P24" t="str">
         <f>CONCATENATE(".db #$", C24, B24, ", #%", IF(E24="R", "0", "1"),  DEC2BIN(D24-1,2), VLOOKUP(F24, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G24, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$D5, #%11100100</v>
+        <v>.db #$26, #%00000100</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
@@ -12558,10 +12554,10 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
@@ -12574,7 +12570,7 @@
       </c>
       <c r="P25" t="str">
         <f>CONCATENATE(".db #$", C25, B25, ", #%", IF(E25="R", "0", "1"),  DEC2BIN(D25-1,2), VLOOKUP(F25, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G25, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$26, #%00000100</v>
+        <v>.db #$46, #%01000100</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
@@ -12582,10 +12578,10 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
         <v>17</v>
@@ -12598,18 +12594,18 @@
       </c>
       <c r="P26" t="str">
         <f>CONCATENATE(".db #$", C26, B26, ", #%", IF(E26="R", "0", "1"),  DEC2BIN(D26-1,2), VLOOKUP(F26, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G26, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$46, #%01000100</v>
+        <v>.db #$76, #%01100100</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>6</v>
       </c>
-      <c r="C27">
-        <v>7</v>
+      <c r="C27" t="s">
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
@@ -12622,15 +12618,15 @@
       </c>
       <c r="P27" t="str">
         <f>CONCATENATE(".db #$", C27, B27, ", #%", IF(E27="R", "0", "1"),  DEC2BIN(D27-1,2), VLOOKUP(F27, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G27, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$76, #%01100100</v>
+        <v>.db #$C6, #%00000100</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -12646,7 +12642,7 @@
       </c>
       <c r="P28" t="str">
         <f>CONCATENATE(".db #$", C28, B28, ", #%", IF(E28="R", "0", "1"),  DEC2BIN(D28-1,2), VLOOKUP(F28, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G28, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$C6, #%00000100</v>
+        <v>.db #$17, #%00000100</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
@@ -12654,10 +12650,10 @@
         <v>7</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
         <v>17</v>
@@ -12670,7 +12666,7 @@
       </c>
       <c r="P29" t="str">
         <f>CONCATENATE(".db #$", C29, B29, ", #%", IF(E29="R", "0", "1"),  DEC2BIN(D29-1,2), VLOOKUP(F29, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G29, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$17, #%00000100</v>
+        <v>.db #$37, #%01100100</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
@@ -12678,10 +12674,10 @@
         <v>7</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
@@ -12694,18 +12690,18 @@
       </c>
       <c r="P30" t="str">
         <f>CONCATENATE(".db #$", C30, B30, ", #%", IF(E30="R", "0", "1"),  DEC2BIN(D30-1,2), VLOOKUP(F30, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G30, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$37, #%01100100</v>
+        <v>.db #$77, #%01000100</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>7</v>
       </c>
-      <c r="C31">
-        <v>7</v>
+      <c r="C31" t="s">
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>17</v>
@@ -12718,18 +12714,18 @@
       </c>
       <c r="P31" t="str">
         <f>CONCATENATE(".db #$", C31, B31, ", #%", IF(E31="R", "0", "1"),  DEC2BIN(D31-1,2), VLOOKUP(F31, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G31, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$77, #%01000100</v>
+        <v>.db #$B7, #%00000100</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
         <v>17</v>
@@ -12742,7 +12738,7 @@
       </c>
       <c r="P32" t="str">
         <f>CONCATENATE(".db #$", C32, B32, ", #%", IF(E32="R", "0", "1"),  DEC2BIN(D32-1,2), VLOOKUP(F32, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G32, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$B7, #%00000100</v>
+        <v>.db #$18, #%01100100</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
@@ -12750,7 +12746,7 @@
         <v>8</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -12766,7 +12762,7 @@
       </c>
       <c r="P33" t="str">
         <f>CONCATENATE(".db #$", C33, B33, ", #%", IF(E33="R", "0", "1"),  DEC2BIN(D33-1,2), VLOOKUP(F33, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G33, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$18, #%01100100</v>
+        <v>.db #$58, #%01100100</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
@@ -12774,7 +12770,7 @@
         <v>8</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -12790,30 +12786,6 @@
       </c>
       <c r="P34" t="str">
         <f>CONCATENATE(".db #$", C34, B34, ", #%", IF(E34="R", "0", "1"),  DEC2BIN(D34-1,2), VLOOKUP(F34, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G34, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$58, #%01100100</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35">
-        <v>8</v>
-      </c>
-      <c r="C35">
-        <v>9</v>
-      </c>
-      <c r="D35">
-        <v>4</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" t="s">
-        <v>4</v>
-      </c>
-      <c r="G35" t="s">
-        <v>26</v>
-      </c>
-      <c r="P35" t="str">
-        <f>CONCATENATE(".db #$", C35, B35, ", #%", IF(E35="R", "0", "1"),  DEC2BIN(D35-1,2), VLOOKUP(F35, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G35, info!$K$5:$L$11, 2, FALSE))</f>
         <v>.db #$98, #%01100100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed level 17, fixed cyan move block bug
</commit_message>
<xml_diff>
--- a/ext_assets/LevelDesign.xlsx
+++ b/ext_assets/LevelDesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nesdev\repos\crillion-nes\crillion-nes\ext_assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85CB5AC-A951-4271-8B95-ADDE65803736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01E97ED-E4C8-451A-87DC-A1DE841D6043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="13" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="18" xr2:uid="{E8D8F587-BDBE-423A-95AF-6E9B76766DB8}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="6" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5182" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5183" uniqueCount="36">
   <si>
     <t>D</t>
   </si>
@@ -1104,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="401">
+  <cellXfs count="397">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2252,16 +2252,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2270,8 +2260,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFAFAF"/>
       <color rgb="FFE2A2F4"/>
-      <color rgb="FFFFAFAF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -7666,7 +7656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D6449E-BDD8-47F1-8C6B-F5B8184718A5}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P34" sqref="P14:P34"/>
     </sheetView>
@@ -11985,11 +11975,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="398"/>
-      <c r="D3" s="399"/>
-      <c r="E3" s="398"/>
-      <c r="F3" s="397"/>
-      <c r="G3" s="397"/>
+      <c r="C3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="44" t="s">
         <v>4</v>
       </c>
@@ -12002,9 +11991,9 @@
       <c r="K3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="397"/>
-      <c r="M3" s="398"/>
-      <c r="N3" s="398"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12012,20 +12001,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="398"/>
-      <c r="D4" s="398"/>
-      <c r="E4" s="398"/>
-      <c r="F4" s="398"/>
-      <c r="G4" s="398"/>
-      <c r="H4" s="398"/>
-      <c r="I4" s="400" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="286" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="400"/>
-      <c r="K4" s="398"/>
-      <c r="L4" s="398"/>
-      <c r="M4" s="398"/>
-      <c r="N4" s="398"/>
+      <c r="J4" s="286"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12033,18 +12022,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="398"/>
-      <c r="D5" s="398"/>
-      <c r="E5" s="398"/>
-      <c r="F5" s="398"/>
-      <c r="G5" s="398"/>
-      <c r="H5" s="398"/>
-      <c r="I5" s="398"/>
-      <c r="J5" s="398"/>
-      <c r="K5" s="398"/>
-      <c r="L5" s="398"/>
-      <c r="M5" s="398"/>
-      <c r="N5" s="398"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12052,18 +12041,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="398"/>
-      <c r="D6" s="398"/>
-      <c r="E6" s="398"/>
-      <c r="F6" s="398"/>
-      <c r="G6" s="398"/>
-      <c r="H6" s="398"/>
-      <c r="I6" s="398"/>
-      <c r="J6" s="398"/>
-      <c r="K6" s="398"/>
-      <c r="L6" s="398"/>
-      <c r="M6" s="398"/>
-      <c r="N6" s="398"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -12120,11 +12109,11 @@
       <c r="B8" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="398"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="398"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="16" t="s">
         <v>4</v>
       </c>
@@ -12146,7 +12135,7 @@
       <c r="L8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="398"/>
+      <c r="M8" s="5"/>
       <c r="N8" s="202" t="s">
         <v>4</v>
       </c>
@@ -12164,7 +12153,7 @@
       <c r="C9" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="398"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="16" t="s">
         <v>4</v>
       </c>
@@ -12186,11 +12175,11 @@
       <c r="K9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="398"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="398"/>
+      <c r="N9" s="5"/>
       <c r="O9" s="210" t="s">
         <v>4</v>
       </c>
@@ -14329,9 +14318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEC0477-6F56-4B92-B5AE-3EF26F62000D}">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14:P64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14627,13 +14616,13 @@
       <c r="F7" s="167" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="167" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="117" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="118" t="s">
+      <c r="G7" s="142" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="315" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="312" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="118" t="s">
@@ -14671,17 +14660,19 @@
       <c r="E8" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="119" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="117" t="s">
+      <c r="F8" s="118" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="117" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="118" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="117" t="s">
+      <c r="J8" s="118" t="s">
         <v>5</v>
       </c>
       <c r="K8" s="119" t="s">
@@ -14715,13 +14706,13 @@
       <c r="F9" s="165" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="117" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="118" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="118" t="s">
+      <c r="G9" s="168" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="170" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="170" t="s">
         <v>5</v>
       </c>
       <c r="J9" s="323" t="s">
@@ -15626,10 +15617,10 @@
         <v>6</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
@@ -15642,7 +15633,7 @@
       </c>
       <c r="P46" t="str">
         <f>CONCATENATE(".db #$", C46, B46, ", #%", IF(E46="R", "0", "1"),  DEC2BIN(D46-1,2), VLOOKUP(F46, info!$H$5:$I$9, 2, FALSE), VLOOKUP(G46, info!$K$5:$L$11, 2, FALSE))</f>
-        <v>.db #$66, #%00100010</v>
+        <v>.db #$56, #%01000010</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.3">

</xml_diff>